<commit_message>
working on pagination I
</commit_message>
<xml_diff>
--- a/static/file/export.xlsx
+++ b/static/file/export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,6 +669,466 @@
         <v>9900000</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>evan</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Jl. kenanga</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Daerah Khusus Ibukota Jakarta</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>08463746284</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2022-11-02 06:29:26.655375</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>SG005LTR</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2730000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>serena</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>jalanan</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Daerah Khusus Ibukota Jakarta</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Kuala lumpur</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2022-11-03 09:36:50.604001</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>CANIFIL</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dsjfhkfdjankjfs</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>faldhiuagiuga</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Kepulauan Riau</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>adfjgfjhivdk</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3246732487246</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2022-11-03 09:53:56.648287</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>FP001DUS</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>10</v>
+      </c>
+      <c r="J8" t="n">
+        <v>62000000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Clara</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Jl ember no 12</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bengkulu</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Jayapura</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>098347724</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2022-11-03 09:55:27.354454</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>SG005LTR</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3640000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ada dnk</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>jl djhdajkbu</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Kepulauan Bangka Belitung</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bengkulu</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0846375673</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2022-11-03 09:56:06.749003</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>SG001DUS</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" t="n">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>kiki</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>jl senang</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Jawa Timur</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Surabaya</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>084757672</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2022-11-03 09:56:33.227591</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>SG001LTR</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1450000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Saartika dewi</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jl merdeka</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Jawa Barat</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bandung</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0873645273</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2022-11-03 09:57:07.941687</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>MFFF1C1</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5400000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>java</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Jl. kenanga</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Nusa Tenggara Barat</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>adfjgfjhivdk</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>3246732487246</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2022-11-03 10:28:02.955195</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>FL007KG</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2240000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>lala</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>lalaland</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Papua Tengah</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>NYC</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>01182734</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2022-11-03 10:35:53</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>SG001DUS</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" t="n">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>cathrine</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>faldhiuagiuga</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bali</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>92378374</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2022-11-03 10:37</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>SG001LTR</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>4</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1160000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
make a little change
</commit_message>
<xml_diff>
--- a/static/file/export.xlsx
+++ b/static/file/export.xlsx
@@ -487,186 +487,186 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sizumi</t>
+          <t>Naomi clara</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Country Road</t>
+          <t>Jl. merdeka no 17</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sumatra Barat</t>
+          <t>Jawa Tengah</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Country road</t>
+          <t>Semarang</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1127446395</t>
+          <t>08963764826</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2022-11-08 06:16</t>
+          <t>2022-11-10 20:26</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>MFFF1C1</t>
+          <t>SG005LTR</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" t="n">
-        <v>16200000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nia Hizkia Pangaribuan</t>
+          <t>Lestari</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jl. merdeka no 17</t>
+          <t>cilandak</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sumatra Utara</t>
+          <t>Daerah Khusus Ibukota Jakarta</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Jakarta</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>08964384729</t>
+          <t>39480579170</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2022-11-10 20:26</t>
+          <t>2022-11-10 00:00:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>SG005LTR</t>
+          <t>FL007KG</t>
         </is>
       </c>
       <c r="I3" t="n">
         <v>3</v>
       </c>
       <c r="J3" t="n">
-        <v>2730000</v>
+        <v>6720000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Naomi</t>
+          <t>Nuvo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jl. merdeka no 17</t>
+          <t>faldhiuagiuga</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jawa Tengah</t>
+          <t>Daerah Khusus Ibukota Jakarta</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Semarang</t>
+          <t>Jakarta</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>08963764826</t>
+          <t>08964384729</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2022-11-10 20:26</t>
+          <t>2022-11-11 00:00:00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>FP500TBT</t>
+          <t>FL007KG</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J4" t="n">
-        <v>3750000</v>
+        <v>22400000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lestari</t>
+          <t>Jeremi</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>cilandak</t>
+          <t>Balik Papan</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Daerah Khusus Ibukota Jakarta</t>
+          <t>Kalimantan Selatan</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jakarta</t>
+          <t>Balik Papan</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>39480579170</t>
+          <t>0897463532</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2022-11-10 00:00:00</t>
+          <t>2022-11-11 00:00:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>FL007KG</t>
+          <t>MFHF1C1</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>6720000</v>
+        <v>2130000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>